<commit_message>
todos los scripts actualizado a cafee_dea y nuevos datos del servidor
</commit_message>
<xml_diff>
--- a/simulations/cobb_douglas_XnY1/scenarios/secenarios_lanzados.xlsx
+++ b/simulations/cobb_douglas_XnY1/scenarios/secenarios_lanzados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Documents\Cafee\simulations\cobb_douglas_XnY1\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83603A7E-0190-4D8E-BE48-7A088BC6D305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC36F59-0990-49A5-9948-3D2C47866187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="7">
   <si>
     <t>nX</t>
   </si>
@@ -44,12 +44,15 @@
   <si>
     <t>cafee_bdea</t>
   </si>
+  <si>
+    <t>x</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,13 +60,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -87,9 +108,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,7 +408,7 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,7 +438,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2">
@@ -412,9 +447,15 @@
       <c r="C2">
         <v>0</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3">
@@ -423,9 +464,15 @@
       <c r="C3">
         <v>0.02</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
       <c r="B4">
@@ -434,9 +481,15 @@
       <c r="C4">
         <v>0.05</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>1</v>
       </c>
       <c r="B5">
@@ -445,9 +498,15 @@
       <c r="C5">
         <v>0</v>
       </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="4">
         <v>1</v>
       </c>
       <c r="B6">
@@ -456,9 +515,15 @@
       <c r="C6">
         <v>0.02</v>
       </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="4">
         <v>1</v>
       </c>
       <c r="B7">
@@ -467,9 +532,15 @@
       <c r="C7">
         <v>0.05</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>1</v>
       </c>
       <c r="B8">
@@ -478,9 +549,15 @@
       <c r="C8">
         <v>0</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="4">
         <v>1</v>
       </c>
       <c r="B9">
@@ -489,9 +566,15 @@
       <c r="C9">
         <v>0.02</v>
       </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="4">
         <v>1</v>
       </c>
       <c r="B10">
@@ -500,9 +583,15 @@
       <c r="C10">
         <v>0.05</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="4">
         <v>1</v>
       </c>
       <c r="B11">
@@ -511,9 +600,13 @@
       <c r="C11">
         <v>0</v>
       </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="4">
         <v>1</v>
       </c>
       <c r="B12">
@@ -522,9 +615,13 @@
       <c r="C12">
         <v>0.02</v>
       </c>
+      <c r="D12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="5">
         <v>1</v>
       </c>
       <c r="B13" s="1">
@@ -533,12 +630,14 @@
       <c r="C13" s="1">
         <v>0.05</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="D13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="3"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="4">
         <v>3</v>
       </c>
       <c r="B14">
@@ -547,9 +646,15 @@
       <c r="C14">
         <v>0</v>
       </c>
+      <c r="D14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="4">
         <v>3</v>
       </c>
       <c r="B15">
@@ -558,9 +663,11 @@
       <c r="C15">
         <v>0.02</v>
       </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="4">
         <v>3</v>
       </c>
       <c r="B16">
@@ -569,9 +676,11 @@
       <c r="C16">
         <v>0.05</v>
       </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="4">
         <v>3</v>
       </c>
       <c r="B17">
@@ -580,9 +689,13 @@
       <c r="C17">
         <v>0</v>
       </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="4">
         <v>3</v>
       </c>
       <c r="B18">
@@ -591,9 +704,13 @@
       <c r="C18">
         <v>0.02</v>
       </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="4">
         <v>3</v>
       </c>
       <c r="B19">
@@ -602,9 +719,13 @@
       <c r="C19">
         <v>0.05</v>
       </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="4">
         <v>3</v>
       </c>
       <c r="B20">
@@ -613,9 +734,13 @@
       <c r="C20">
         <v>0</v>
       </c>
+      <c r="D20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="4">
         <v>3</v>
       </c>
       <c r="B21">
@@ -624,9 +749,13 @@
       <c r="C21">
         <v>0.02</v>
       </c>
+      <c r="D21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="4">
         <v>3</v>
       </c>
       <c r="B22">
@@ -635,9 +764,13 @@
       <c r="C22">
         <v>0.05</v>
       </c>
+      <c r="D22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="4">
         <v>3</v>
       </c>
       <c r="B23">
@@ -646,9 +779,13 @@
       <c r="C23">
         <v>0</v>
       </c>
+      <c r="D23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="4">
         <v>3</v>
       </c>
       <c r="B24">
@@ -657,9 +794,13 @@
       <c r="C24">
         <v>0.02</v>
       </c>
+      <c r="D24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="5">
         <v>3</v>
       </c>
       <c r="B25" s="1">
@@ -668,12 +809,14 @@
       <c r="C25" s="1">
         <v>0.05</v>
       </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="D25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="3"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="4">
         <v>6</v>
       </c>
       <c r="B26">
@@ -682,9 +825,11 @@
       <c r="C26">
         <v>0</v>
       </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="4">
         <v>6</v>
       </c>
       <c r="B27">
@@ -693,9 +838,11 @@
       <c r="C27">
         <v>0.02</v>
       </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="4">
         <v>6</v>
       </c>
       <c r="B28">
@@ -704,9 +851,11 @@
       <c r="C28">
         <v>0.05</v>
       </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="4">
         <v>6</v>
       </c>
       <c r="B29">
@@ -715,9 +864,11 @@
       <c r="C29">
         <v>0</v>
       </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="4">
         <v>6</v>
       </c>
       <c r="B30">
@@ -726,9 +877,11 @@
       <c r="C30">
         <v>0.02</v>
       </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="4">
         <v>6</v>
       </c>
       <c r="B31">
@@ -737,9 +890,11 @@
       <c r="C31">
         <v>0.05</v>
       </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="4">
         <v>6</v>
       </c>
       <c r="B32">
@@ -748,9 +903,11 @@
       <c r="C32">
         <v>0</v>
       </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="4">
         <v>6</v>
       </c>
       <c r="B33">
@@ -759,9 +916,11 @@
       <c r="C33">
         <v>0.02</v>
       </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="4">
         <v>6</v>
       </c>
       <c r="B34">
@@ -770,9 +929,11 @@
       <c r="C34">
         <v>0.05</v>
       </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="4">
         <v>6</v>
       </c>
       <c r="B35">
@@ -781,9 +942,11 @@
       <c r="C35">
         <v>0</v>
       </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="4">
         <v>6</v>
       </c>
       <c r="B36">
@@ -792,9 +955,11 @@
       <c r="C36">
         <v>0.02</v>
       </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+      <c r="A37" s="5">
         <v>6</v>
       </c>
       <c r="B37" s="1">
@@ -803,12 +968,12 @@
       <c r="C37" s="1">
         <v>0.05</v>
       </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" s="4">
         <v>9</v>
       </c>
       <c r="B38">
@@ -817,9 +982,13 @@
       <c r="C38">
         <v>0</v>
       </c>
+      <c r="D38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="4">
         <v>9</v>
       </c>
       <c r="B39">
@@ -828,9 +997,13 @@
       <c r="C39">
         <v>0.02</v>
       </c>
+      <c r="D39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="4">
         <v>9</v>
       </c>
       <c r="B40">
@@ -839,9 +1012,13 @@
       <c r="C40">
         <v>0.05</v>
       </c>
+      <c r="D40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" s="4">
         <v>9</v>
       </c>
       <c r="B41">
@@ -850,9 +1027,13 @@
       <c r="C41">
         <v>0</v>
       </c>
+      <c r="D41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" s="4">
         <v>9</v>
       </c>
       <c r="B42">
@@ -861,9 +1042,13 @@
       <c r="C42">
         <v>0.02</v>
       </c>
+      <c r="D42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="2"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="A43" s="4">
         <v>9</v>
       </c>
       <c r="B43">
@@ -872,9 +1057,13 @@
       <c r="C43">
         <v>0.05</v>
       </c>
+      <c r="D43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="2"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="A44" s="4">
         <v>9</v>
       </c>
       <c r="B44">
@@ -883,9 +1072,13 @@
       <c r="C44">
         <v>0</v>
       </c>
+      <c r="D44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="A45" s="4">
         <v>9</v>
       </c>
       <c r="B45">
@@ -894,9 +1087,13 @@
       <c r="C45">
         <v>0.02</v>
       </c>
+      <c r="D45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" s="4">
         <v>9</v>
       </c>
       <c r="B46">
@@ -905,9 +1102,13 @@
       <c r="C46">
         <v>0.05</v>
       </c>
+      <c r="D46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="A47" s="4">
         <v>9</v>
       </c>
       <c r="B47">
@@ -916,9 +1117,13 @@
       <c r="C47">
         <v>0</v>
       </c>
+      <c r="D47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="A48" s="4">
         <v>9</v>
       </c>
       <c r="B48">
@@ -927,9 +1132,13 @@
       <c r="C48">
         <v>0.02</v>
       </c>
+      <c r="D48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+      <c r="A49" s="5">
         <v>9</v>
       </c>
       <c r="B49" s="1">
@@ -938,12 +1147,14 @@
       <c r="C49" s="1">
         <v>0.05</v>
       </c>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
+      <c r="D49" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" s="3"/>
       <c r="F49" s="1"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="A50" s="4">
         <v>12</v>
       </c>
       <c r="B50">
@@ -952,9 +1163,15 @@
       <c r="C50">
         <v>0</v>
       </c>
+      <c r="D50" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" s="4">
         <v>12</v>
       </c>
       <c r="B51">
@@ -963,9 +1180,15 @@
       <c r="C51">
         <v>0.02</v>
       </c>
+      <c r="D51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" s="4">
         <v>12</v>
       </c>
       <c r="B52">
@@ -974,9 +1197,15 @@
       <c r="C52">
         <v>0.05</v>
       </c>
+      <c r="D52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="A53" s="4">
         <v>12</v>
       </c>
       <c r="B53">
@@ -985,9 +1214,15 @@
       <c r="C53">
         <v>0</v>
       </c>
+      <c r="D53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="A54" s="4">
         <v>12</v>
       </c>
       <c r="B54">
@@ -996,9 +1231,15 @@
       <c r="C54">
         <v>0.02</v>
       </c>
+      <c r="D54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="A55" s="4">
         <v>12</v>
       </c>
       <c r="B55">
@@ -1007,9 +1248,15 @@
       <c r="C55">
         <v>0.05</v>
       </c>
+      <c r="D55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="A56" s="4">
         <v>12</v>
       </c>
       <c r="B56">
@@ -1018,9 +1265,15 @@
       <c r="C56">
         <v>0</v>
       </c>
+      <c r="D56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="A57" s="4">
         <v>12</v>
       </c>
       <c r="B57">
@@ -1029,9 +1282,15 @@
       <c r="C57">
         <v>0.02</v>
       </c>
+      <c r="D57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="A58" s="4">
         <v>12</v>
       </c>
       <c r="B58">
@@ -1040,9 +1299,13 @@
       <c r="C58">
         <v>0.05</v>
       </c>
+      <c r="D58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="A59" s="4">
         <v>12</v>
       </c>
       <c r="B59">
@@ -1051,9 +1314,15 @@
       <c r="C59">
         <v>0</v>
       </c>
+      <c r="D59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="A60" s="4">
         <v>12</v>
       </c>
       <c r="B60">
@@ -1062,9 +1331,13 @@
       <c r="C60">
         <v>0.02</v>
       </c>
+      <c r="D60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" s="2"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
+      <c r="A61" s="5">
         <v>12</v>
       </c>
       <c r="B61" s="1">
@@ -1073,11 +1346,14 @@
       <c r="C61" s="1">
         <v>0.05</v>
       </c>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
+      <c r="D61" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" s="3"/>
       <c r="F61" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
añadir cuantos modelos fallan
</commit_message>
<xml_diff>
--- a/simulations/cobb_douglas_XnY1/scenarios/secenarios_lanzados.xlsx
+++ b/simulations/cobb_douglas_XnY1/scenarios/secenarios_lanzados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Documents\Cafee\simulations\cobb_douglas_XnY1\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC36F59-0990-49A5-9948-3D2C47866187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335D516A-70D2-4DA2-9712-D120C9291CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -407,8 +407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
arreglo cafee dea y bdea con trycatch
</commit_message>
<xml_diff>
--- a/simulations/cobb_douglas_XnY1/scenarios/secenarios_lanzados.xlsx
+++ b/simulations/cobb_douglas_XnY1/scenarios/secenarios_lanzados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://miumh-my.sharepoint.com/personal/ricardo_gonzalezm_miumh_umh_es/Documents/Documentos/Cafee/simulations/cobb_douglas_XnY1/scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{C802BF86-7A38-4F14-9EB6-7B5F3C7DCF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{100FD6BB-8D0B-4518-BAEF-27FCCD9B52FF}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{C802BF86-7A38-4F14-9EB6-7B5F3C7DCF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B486EE1-F985-430A-A3DF-6FE9E5EEA6B6}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="7">
   <si>
     <t>nX</t>
   </si>
@@ -131,6 +131,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -398,8 +402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,9 +445,7 @@
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -458,9 +460,7 @@
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -475,9 +475,7 @@
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -492,9 +490,7 @@
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -509,9 +505,7 @@
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -526,9 +520,7 @@
       <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
@@ -543,9 +535,7 @@
       <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -560,9 +550,7 @@
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -577,9 +565,7 @@
       <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -640,9 +626,7 @@
       <c r="D14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
@@ -657,9 +641,7 @@
       <c r="D15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
@@ -674,9 +656,7 @@
       <c r="D16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
@@ -824,7 +804,9 @@
       <c r="C26">
         <v>0</v>
       </c>
-      <c r="D26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -837,7 +819,9 @@
       <c r="C27">
         <v>0.02</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -850,7 +834,9 @@
       <c r="C28">
         <v>0.05</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -863,7 +849,9 @@
       <c r="C29">
         <v>0</v>
       </c>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -876,7 +864,9 @@
       <c r="C30">
         <v>0.02</v>
       </c>
-      <c r="D30" s="2"/>
+      <c r="D30" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -889,7 +879,9 @@
       <c r="C31">
         <v>0.05</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -902,7 +894,9 @@
       <c r="C32">
         <v>0</v>
       </c>
-      <c r="D32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -915,7 +909,9 @@
       <c r="C33">
         <v>0.02</v>
       </c>
-      <c r="D33" s="2"/>
+      <c r="D33" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -928,7 +924,9 @@
       <c r="C34">
         <v>0.05</v>
       </c>
-      <c r="D34" s="2"/>
+      <c r="D34" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -941,7 +939,9 @@
       <c r="C35">
         <v>0</v>
       </c>
-      <c r="D35" s="2"/>
+      <c r="D35" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -954,7 +954,9 @@
       <c r="C36">
         <v>0.02</v>
       </c>
-      <c r="D36" s="2"/>
+      <c r="D36" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -967,7 +969,9 @@
       <c r="C37" s="1">
         <v>0.05</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E37" s="3"/>
       <c r="F37" s="1"/>
     </row>
@@ -984,9 +988,7 @@
       <c r="D38" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
@@ -1001,9 +1003,7 @@
       <c r="D39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
@@ -1018,9 +1018,7 @@
       <c r="D40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
@@ -1171,9 +1169,7 @@
       <c r="D50" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E50" s="2"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
@@ -1188,9 +1184,7 @@
       <c r="D51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E51" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
@@ -1205,9 +1199,7 @@
       <c r="D52" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
@@ -1222,9 +1214,7 @@
       <c r="D53" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E53" s="2"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
@@ -1239,9 +1229,7 @@
       <c r="D54" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E54" s="2"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
@@ -1256,9 +1244,7 @@
       <c r="D55" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E55" s="2"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
@@ -1273,9 +1259,7 @@
       <c r="D56" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E56" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
@@ -1290,9 +1274,7 @@
       <c r="D57" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E57" s="2"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
@@ -1322,9 +1304,7 @@
       <c r="D59" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E59" s="2"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="4">

</xml_diff>